<commit_message>
Add a new test case
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Feliciano\Documents\workspace\utility\ConfigTool\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Feliciano\Documents\workspace\utility\Xlsx2Json\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9675" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9675" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="weaponStuffs" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,8 @@
     <sheet name="shieldStuffs" sheetId="4" r:id="rId4"/>
     <sheet name="essenceFragmentStuffs" sheetId="6" r:id="rId5"/>
     <sheet name="bottleStuffs" sheetId="5" r:id="rId6"/>
+    <sheet name="map" sheetId="7" r:id="rId7"/>
+    <sheet name="monster" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -29,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="105">
   <si>
     <t>_id</t>
   </si>
@@ -226,9 +228,6 @@
     <t>22,15,10,0.12</t>
   </si>
   <si>
-    <t>25, 20, 15,0.01</t>
-  </si>
-  <si>
     <t>COPPER_SHIELD</t>
   </si>
   <si>
@@ -257,13 +256,103 @@
   </si>
   <si>
     <t>BLOOD</t>
+  </si>
+  <si>
+    <t>_class</t>
+  </si>
+  <si>
+    <t>stage</t>
+  </si>
+  <si>
+    <t>floor</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>centaurs.game.vocalwarrior.business.entity.map.Map</t>
+  </si>
+  <si>
+    <t>monsterInScene</t>
+  </si>
+  <si>
+    <t>BASIC</t>
+  </si>
+  <si>
+    <t>STORY</t>
+  </si>
+  <si>
+    <t>REFERENCE</t>
+  </si>
+  <si>
+    <t>Object</t>
+  </si>
+  <si>
+    <t>monsterId</t>
+  </si>
+  <si>
+    <t>power</t>
+  </si>
+  <si>
+    <t>intelligence</t>
+  </si>
+  <si>
+    <t>ai</t>
+  </si>
+  <si>
+    <t>equippedWeaponIds</t>
+  </si>
+  <si>
+    <t>equippedSkillIds</t>
+  </si>
+  <si>
+    <t>goldReward</t>
+  </si>
+  <si>
+    <t>experienceReward</t>
+  </si>
+  <si>
+    <t>diamondReward</t>
+  </si>
+  <si>
+    <t>stuffRewardTypes</t>
+  </si>
+  <si>
+    <t>weaponRewardId</t>
+  </si>
+  <si>
+    <t>skillRewardId</t>
+  </si>
+  <si>
+    <t>essenceRewardId</t>
+  </si>
+  <si>
+    <t>ARRAY&lt;STRING&gt;</t>
+  </si>
+  <si>
+    <t>CHIEF</t>
+  </si>
+  <si>
+    <t>Chief</t>
+  </si>
+  <si>
+    <t>KICK,PUNCH</t>
+  </si>
+  <si>
+    <t>mapid</t>
+  </si>
+  <si>
+    <t>monster@monster#monsterId</t>
+  </si>
+  <si>
+    <t>$numberLong: "1", testatt1:true, testatt2:abc123, testatt3:"aaa", testatt4:""</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -274,6 +363,14 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -302,16 +399,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -593,7 +693,7 @@
   <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD4"/>
+      <selection activeCell="N1" sqref="N1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -948,7 +1048,7 @@
   <dimension ref="A1:P3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1086,9 +1186,6 @@
       </c>
       <c r="J3" t="s">
         <v>64</v>
-      </c>
-      <c r="K3" t="s">
-        <v>65</v>
       </c>
       <c r="L3">
         <v>18</v>
@@ -1181,7 +1278,7 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B3" t="b">
         <v>1</v>
@@ -1190,16 +1287,16 @@
         <v>3600</v>
       </c>
       <c r="D3" t="s">
+        <v>66</v>
+      </c>
+      <c r="E3" t="s">
         <v>67</v>
-      </c>
-      <c r="E3" t="s">
-        <v>68</v>
       </c>
       <c r="F3" t="s">
         <v>42</v>
       </c>
       <c r="G3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H3">
         <v>100</v>
@@ -1286,10 +1383,10 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>69</v>
+      </c>
+      <c r="B3" t="s">
         <v>70</v>
-      </c>
-      <c r="B3" t="s">
-        <v>71</v>
       </c>
       <c r="C3">
         <v>6000</v>
@@ -1298,7 +1395,7 @@
         <v>40</v>
       </c>
       <c r="E3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F3" t="s">
         <v>42</v>
@@ -1323,7 +1420,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
@@ -1398,19 +1495,19 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B3" t="s">
         <v>73</v>
-      </c>
-      <c r="B3" t="s">
-        <v>74</v>
       </c>
       <c r="C3">
         <v>6000</v>
       </c>
       <c r="D3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F3" t="s">
         <v>42</v>
@@ -1419,7 +1516,7 @@
         <v>1</v>
       </c>
       <c r="H3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="I3">
         <v>50</v>
@@ -1432,4 +1529,266 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:H3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="6" width="19" customWidth="1"/>
+    <col min="7" max="7" width="30" customWidth="1"/>
+    <col min="8" max="8" width="19" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>0</v>
+      </c>
+      <c r="B3" t="s">
+        <v>104</v>
+      </c>
+      <c r="C3" t="s">
+        <v>79</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3" t="s">
+        <v>82</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="G2" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:Q3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="17" width="14.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>0</v>
+      </c>
+      <c r="B3" t="s">
+        <v>99</v>
+      </c>
+      <c r="C3" t="s">
+        <v>100</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3">
+        <v>100</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>1</v>
+      </c>
+      <c r="I3" t="s">
+        <v>101</v>
+      </c>
+      <c r="K3">
+        <v>100</v>
+      </c>
+      <c r="L3">
+        <v>100</v>
+      </c>
+      <c r="M3">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Add some more test cases
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9675" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9675" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="weaponStuffs" sheetId="1" r:id="rId1"/>
@@ -1047,7 +1047,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
@@ -1535,8 +1535,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:H3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1637,7 +1637,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>

<commit_message>
Fixed a type identify bug and replaced the test file
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -168,9 +168,6 @@
     <t>Array&lt;String&gt;</t>
   </si>
   <si>
-    <t>Array&lt;Float&gt;</t>
-  </si>
-  <si>
     <t>BIG_SWORD</t>
   </si>
   <si>
@@ -346,6 +343,9 @@
   </si>
   <si>
     <t>$numberLong: "1", testatt1:true, testatt2:abc123, testatt3:"aaa", testatt4:""</t>
+  </si>
+  <si>
+    <t>Array&lt;Double&gt;</t>
   </si>
 </sst>
 </file>
@@ -785,10 +785,10 @@
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B3" t="s">
         <v>46</v>
-      </c>
-      <c r="B3" t="s">
-        <v>47</v>
       </c>
       <c r="C3">
         <v>0</v>
@@ -797,7 +797,7 @@
         <v>40</v>
       </c>
       <c r="E3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F3" t="s">
         <v>42</v>
@@ -845,67 +845,67 @@
   <sheetData>
     <row r="1" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="O1" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="P1" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="Q1" s="2" t="s">
         <v>44</v>
       </c>
       <c r="R1" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="S1" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="T1" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="U1" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -975,16 +975,16 @@
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B3" t="b">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3" t="s">
         <v>50</v>
-      </c>
-      <c r="B3" t="b">
-        <v>0</v>
-      </c>
-      <c r="C3">
-        <v>0</v>
-      </c>
-      <c r="D3" t="s">
-        <v>51</v>
       </c>
       <c r="E3" t="s">
         <v>40</v>
@@ -993,10 +993,10 @@
         <v>42</v>
       </c>
       <c r="G3" t="s">
+        <v>51</v>
+      </c>
+      <c r="H3" t="s">
         <v>52</v>
-      </c>
-      <c r="H3" t="s">
-        <v>53</v>
       </c>
       <c r="I3">
         <v>30</v>
@@ -1014,22 +1014,22 @@
         <v>200</v>
       </c>
       <c r="N3" t="s">
+        <v>53</v>
+      </c>
+      <c r="O3" t="s">
         <v>54</v>
-      </c>
-      <c r="O3" t="s">
-        <v>55</v>
       </c>
       <c r="P3">
         <v>60</v>
       </c>
       <c r="Q3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="R3">
         <v>1000</v>
       </c>
       <c r="S3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="T3">
         <v>10</v>
@@ -1048,7 +1048,7 @@
   <dimension ref="A1:P3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+      <selection activeCell="L18" sqref="L18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1085,10 +1085,10 @@
         <v>44</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>45</v>
+        <v>104</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>45</v>
+        <v>104</v>
       </c>
       <c r="L1" s="2" t="s">
         <v>36</v>
@@ -1158,34 +1158,34 @@
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>57</v>
+      </c>
+      <c r="B3" t="b">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3" t="s">
         <v>58</v>
-      </c>
-      <c r="B3" t="b">
-        <v>0</v>
-      </c>
-      <c r="C3">
-        <v>0</v>
-      </c>
-      <c r="D3" t="s">
-        <v>59</v>
       </c>
       <c r="E3" t="s">
         <v>40</v>
       </c>
       <c r="F3" t="s">
+        <v>59</v>
+      </c>
+      <c r="G3" t="s">
         <v>60</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>61</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
         <v>62</v>
       </c>
-      <c r="I3" t="s">
+      <c r="J3" t="s">
         <v>63</v>
-      </c>
-      <c r="J3" t="s">
-        <v>64</v>
       </c>
       <c r="L3">
         <v>18</v>
@@ -1278,7 +1278,7 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B3" t="b">
         <v>1</v>
@@ -1287,16 +1287,16 @@
         <v>3600</v>
       </c>
       <c r="D3" t="s">
+        <v>65</v>
+      </c>
+      <c r="E3" t="s">
         <v>66</v>
-      </c>
-      <c r="E3" t="s">
-        <v>67</v>
       </c>
       <c r="F3" t="s">
         <v>42</v>
       </c>
       <c r="G3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H3">
         <v>100</v>
@@ -1383,10 +1383,10 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B3" t="s">
         <v>69</v>
-      </c>
-      <c r="B3" t="s">
-        <v>70</v>
       </c>
       <c r="C3">
         <v>6000</v>
@@ -1395,7 +1395,7 @@
         <v>40</v>
       </c>
       <c r="E3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F3" t="s">
         <v>42</v>
@@ -1495,19 +1495,19 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>71</v>
+      </c>
+      <c r="B3" t="s">
         <v>72</v>
-      </c>
-      <c r="B3" t="s">
-        <v>73</v>
       </c>
       <c r="C3">
         <v>6000</v>
       </c>
       <c r="D3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F3" t="s">
         <v>42</v>
@@ -1516,7 +1516,7 @@
         <v>1</v>
       </c>
       <c r="H3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I3">
         <v>50</v>
@@ -1548,54 +1548,54 @@
   <sheetData>
     <row r="1" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="2" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="G2" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>103</v>
-      </c>
       <c r="H2" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -1603,10 +1603,10 @@
         <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D3">
         <v>0</v>
@@ -1615,7 +1615,7 @@
         <v>0</v>
       </c>
       <c r="F3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G3">
         <v>0</v>
@@ -1648,60 +1648,60 @@
   <sheetData>
     <row r="1" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="O1" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="P1" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="Q1" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="2" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>0</v>
@@ -1713,43 +1713,43 @@
         <v>17</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>8</v>
       </c>
       <c r="G2" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="H2" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="I2" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="J2" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="K2" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="L2" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="L2" s="1" t="s">
+      <c r="M2" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="M2" s="1" t="s">
+      <c r="N2" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="N2" s="1" t="s">
+      <c r="O2" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="O2" s="1" t="s">
+      <c r="P2" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="P2" s="1" t="s">
+      <c r="Q2" s="1" t="s">
         <v>96</v>
-      </c>
-      <c r="Q2" s="1" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
@@ -1757,10 +1757,10 @@
         <v>0</v>
       </c>
       <c r="B3" t="s">
+        <v>98</v>
+      </c>
+      <c r="C3" t="s">
         <v>99</v>
-      </c>
-      <c r="C3" t="s">
-        <v>100</v>
       </c>
       <c r="D3">
         <v>1</v>
@@ -1778,7 +1778,7 @@
         <v>1</v>
       </c>
       <c r="I3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="K3">
         <v>100</v>

</xml_diff>

<commit_message>
Added an error handler and updated test case
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -9,17 +9,18 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9675" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9675"/>
   </bookViews>
   <sheets>
-    <sheet name="weaponStuffs" sheetId="1" r:id="rId1"/>
-    <sheet name="skillStuffs" sheetId="2" r:id="rId2"/>
-    <sheet name="essenceStuffs" sheetId="3" r:id="rId3"/>
-    <sheet name="shieldStuffs" sheetId="4" r:id="rId4"/>
-    <sheet name="essenceFragmentStuffs" sheetId="6" r:id="rId5"/>
-    <sheet name="bottleStuffs" sheetId="5" r:id="rId6"/>
-    <sheet name="map" sheetId="7" r:id="rId7"/>
-    <sheet name="monster" sheetId="8" r:id="rId8"/>
+    <sheet name="example" sheetId="9" r:id="rId1"/>
+    <sheet name="weaponStuffs" sheetId="1" r:id="rId2"/>
+    <sheet name="skillStuffs" sheetId="2" r:id="rId3"/>
+    <sheet name="essenceStuffs" sheetId="3" r:id="rId4"/>
+    <sheet name="shieldStuffs" sheetId="4" r:id="rId5"/>
+    <sheet name="essenceFragmentStuffs" sheetId="6" r:id="rId6"/>
+    <sheet name="bottleStuffs" sheetId="5" r:id="rId7"/>
+    <sheet name="map" sheetId="7" r:id="rId8"/>
+    <sheet name="monster" sheetId="8" r:id="rId9"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="121">
   <si>
     <t>_id</t>
   </si>
@@ -346,6 +347,54 @@
   </si>
   <si>
     <t>Array&lt;Double&gt;</t>
+  </si>
+  <si>
+    <t>Reference</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>weapon</t>
+  </si>
+  <si>
+    <t>flag</t>
+  </si>
+  <si>
+    <t>nums</t>
+  </si>
+  <si>
+    <t>words</t>
+  </si>
+  <si>
+    <t>objects</t>
+  </si>
+  <si>
+    <t>shiled</t>
+  </si>
+  <si>
+    <t>sword</t>
+  </si>
+  <si>
+    <t>1,2</t>
+  </si>
+  <si>
+    <t>hello,world</t>
+  </si>
+  <si>
+    <t>a:123,b:"45",c:false</t>
+  </si>
+  <si>
+    <t>3,5,8</t>
+  </si>
+  <si>
+    <t>oh god</t>
+  </si>
+  <si>
+    <t>shiled@shieldStuffs#_id</t>
+  </si>
+  <si>
+    <t>a:11,b:"22",c:true</t>
   </si>
 </sst>
 </file>
@@ -690,6 +739,118 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="5" width="17.140625" customWidth="1"/>
+    <col min="6" max="7" width="27.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>123</v>
+      </c>
+      <c r="B3" t="s">
+        <v>112</v>
+      </c>
+      <c r="C3" t="b">
+        <v>1</v>
+      </c>
+      <c r="D3" t="s">
+        <v>114</v>
+      </c>
+      <c r="E3" t="s">
+        <v>115</v>
+      </c>
+      <c r="F3" t="s">
+        <v>64</v>
+      </c>
+      <c r="G3" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>456</v>
+      </c>
+      <c r="B4" t="s">
+        <v>113</v>
+      </c>
+      <c r="C4" t="b">
+        <v>0</v>
+      </c>
+      <c r="D4" t="s">
+        <v>117</v>
+      </c>
+      <c r="E4" t="s">
+        <v>118</v>
+      </c>
+      <c r="G4" t="s">
+        <v>120</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="F2" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -830,7 +991,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U3"/>
   <sheetViews>
@@ -1043,11 +1204,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L18" sqref="L18"/>
     </sheetView>
   </sheetViews>
@@ -1208,15 +1369,18 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.140625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
@@ -1310,7 +1474,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I3"/>
   <sheetViews>
@@ -1416,7 +1580,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J3"/>
   <sheetViews>
@@ -1531,7 +1695,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H3"/>
   <sheetViews>
@@ -1633,7 +1797,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q3"/>
   <sheetViews>

</xml_diff>